<commit_message>
report formatting - refactored
</commit_message>
<xml_diff>
--- a/reports/_ICB_SUMMIT ALLIANCE PORT LIMITED_container_report_2018-11-28_47_.xlsx
+++ b/reports/_ICB_SUMMIT ALLIANCE PORT LIMITED_container_report_2018-11-28_47_.xlsx
@@ -17,9 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
+    <numFmt numFmtId="102" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -108,13 +109,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
     <xf borderId="2" numFmtId="0" fontId="1" fillId="2" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" wrapText="false"/>
     </xf>
+    <xf borderId="0" numFmtId="102" fontId="0" fillId="0" applyNumberFormat="true" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf borderId="3" numFmtId="0" fontId="2" fillId="3" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
   </cellXfs>
   <cellStyles count="1">
@@ -130,43 +132,35 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="75.25617977528091" hidden="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.8561797752809" hidden="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="20.713483146067418"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.713483146067416"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="22.213483146067418"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.713483146067416"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.213483146067418"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.213483146067418"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.213483146067418"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.713483146067418"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.213483146067416"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.213483146067418"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.713483146067418"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="25.213483146067418"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="21.789887640449443"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.213483146067418"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.213483146067418"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.713483146067416"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.213483146067418"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="23.713483146067418"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="14.713483146067416"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="14.713483146067416"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="28.213483146067418"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.213483146067416"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="8.713483146067416"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="20.713483146067418"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.213483146067418"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="19.213483146067418"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="23.713483146067418"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="17.713483146067418"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="16.213483146067418"/>
   </cols>
   <sheetData>
     <row ht="20" customHeight="true" r="1">
@@ -176,220 +170,173 @@
         </is>
       </c>
     </row>
-    <row ht="18" customHeight="true" r="2">
+    <row ht="16" customHeight="true" r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t> KATGHAR, NORTH PATENGA, CHITTAGONG-4204. </t>
-        </is>
-      </c>
-    </row>
-    <row ht="16" customHeight="true" r="3">
+          <t>ICB</t>
+        </is>
+      </c>
+    </row>
+    <row ht="14" customHeight="true" r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>ICB</t>
-        </is>
-      </c>
-    </row>
-    <row ht="14" customHeight="true" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
           <t>In Report</t>
         </is>
       </c>
     </row>
-    <row ht="16" customHeight="true" r="5">
-      <c r="A5" s="4" t="inlineStr">
+    <row ht="16" customHeight="true" r="4">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Total number of conatiners:1</t>
         </is>
       </c>
     </row>
-    <row r="6"/>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Container Number</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Container Size</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>Container Type</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>Current Depot Unit</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>Permitted Depot Unit</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>Mlo</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>Source Location</t>
+        </is>
+      </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>Import Vessel Name</t>
+        </is>
+      </c>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>Import Rotation Number</t>
+        </is>
+      </c>
+      <c r="L6" s="5" t="inlineStr">
+        <is>
+          <t>Gate In Date</t>
+        </is>
+      </c>
+      <c r="M6" s="5" t="inlineStr">
+        <is>
+          <t>Container Condition Name</t>
+        </is>
+      </c>
+      <c r="N6" s="5" t="inlineStr">
+        <is>
+          <t>Di Agent</t>
+        </is>
+      </c>
+      <c r="O6" s="5" t="inlineStr">
+        <is>
+          <t>Di Mlo</t>
+        </is>
+      </c>
+      <c r="P6" s="5" t="inlineStr">
+        <is>
+          <t>Di Date</t>
+        </is>
+      </c>
+      <c r="Q6" s="5" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+      <c r="R6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Area Name</t>
+        </is>
+      </c>
+      <c r="S6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Part Name</t>
+        </is>
+      </c>
+      <c r="T6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Description</t>
+        </is>
+      </c>
+      <c r="U6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Component</t>
+        </is>
+      </c>
+      <c r="V6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Type</t>
+        </is>
+      </c>
+      <c r="W6" s="5" t="inlineStr">
+        <is>
+          <t>Repair Type</t>
+        </is>
+      </c>
+    </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Container Number</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>Company</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>Agent</t>
-        </is>
-      </c>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>MLO</t>
-        </is>
-      </c>
-      <c r="H7" s="4" t="inlineStr">
-        <is>
-          <t>Issue Date</t>
-        </is>
-      </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>In Date</t>
-        </is>
-      </c>
-      <c r="J7" s="4" t="inlineStr">
-        <is>
-          <t>Container Condition</t>
-        </is>
-      </c>
-      <c r="K7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Area</t>
-        </is>
-      </c>
-      <c r="L7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Part</t>
-        </is>
-      </c>
-      <c r="M7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Description</t>
-        </is>
-      </c>
-      <c r="N7" s="4" t="inlineStr">
-        <is>
-          <t>Unstuffing Date</t>
-        </is>
-      </c>
-      <c r="O7" s="4" t="inlineStr">
-        <is>
-          <t>Out Date</t>
-        </is>
-      </c>
-      <c r="P7" s="4" t="inlineStr">
-        <is>
-          <t>Seal Number</t>
-        </is>
-      </c>
-      <c r="Q7" s="4" t="inlineStr">
-        <is>
-          <t>Amended Seal No</t>
-        </is>
-      </c>
-      <c r="R7" s="4" t="inlineStr">
-        <is>
-          <t>Vessel</t>
-        </is>
-      </c>
-      <c r="S7" s="4" t="inlineStr">
-        <is>
-          <t>Rotation #</t>
-        </is>
-      </c>
-      <c r="T7" s="4" t="inlineStr">
-        <is>
-          <t>Line #</t>
-        </is>
-      </c>
-      <c r="U7" s="4" t="inlineStr">
-        <is>
-          <t>BE #</t>
-        </is>
-      </c>
-      <c r="V7" s="4" t="inlineStr">
-        <is>
-          <t>BL #</t>
-        </is>
-      </c>
-      <c r="W7" s="4" t="inlineStr">
-        <is>
-          <t>Location - From</t>
-        </is>
-      </c>
-      <c r="X7" s="4" t="inlineStr">
-        <is>
-          <t>Depo Loc</t>
-        </is>
-      </c>
-      <c r="Y7" s="4" t="inlineStr">
-        <is>
-          <t>Importer</t>
-        </is>
-      </c>
-      <c r="Z7" s="4" t="inlineStr">
-        <is>
-          <t>CNF</t>
-        </is>
-      </c>
-      <c r="AA7" s="4" t="inlineStr">
-        <is>
-          <t>EIR #</t>
-        </is>
-      </c>
-      <c r="AB7" s="4" t="inlineStr">
-        <is>
-          <t>Commodity</t>
-        </is>
-      </c>
-      <c r="AC7" s="4" t="inlineStr">
-        <is>
-          <t>In Transport</t>
-        </is>
-      </c>
-      <c r="AD7" s="4" t="inlineStr">
-        <is>
-          <t>In Trailer</t>
-        </is>
-      </c>
-      <c r="AE7" s="4" t="inlineStr">
-        <is>
-          <t>In Remarks</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0"/>
-      <c r="H8" s="0"/>
-      <c r="I8" s="0"/>
-      <c r="J8" s="0"/>
-      <c r="K8" s="0"/>
-      <c r="L8" s="0" t="d">
+      <c r="A7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0" t="d">
         <v>0001-01-01T00:00:00</v>
       </c>
-      <c r="M8" s="0"/>
-      <c r="N8" s="0"/>
-      <c r="O8" s="0"/>
-      <c r="P8" s="0"/>
-      <c r="Q8" s="0"/>
-      <c r="R8" s="0"/>
-      <c r="S8" s="0"/>
-      <c r="T8" s="0"/>
-      <c r="U8" s="0"/>
-      <c r="V8" s="0"/>
-      <c r="W8" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
@@ -412,23 +359,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="75.25617977528091" hidden="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.8561797752809" hidden="false"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.213483146067416"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.713483146067418"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="10.213483146067416"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="7.213483146067416"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.213483146067416"/>
   </cols>
   <sheetData>
     <row ht="20" customHeight="true" r="1">
@@ -438,106 +385,104 @@
         </is>
       </c>
     </row>
-    <row ht="18" customHeight="true" r="2">
+    <row ht="16" customHeight="true" r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t> KATGHAR, NORTH PATENGA, CHITTAGONG-4204. </t>
-        </is>
-      </c>
-    </row>
-    <row ht="16" customHeight="true" r="3">
+          <t>ICB</t>
+        </is>
+      </c>
+    </row>
+    <row ht="14" customHeight="true" r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>ICB</t>
-        </is>
-      </c>
-    </row>
-    <row ht="14" customHeight="true" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
           <t>In Report Summary</t>
         </is>
       </c>
     </row>
-    <row r="5"/>
+    <row r="4"/>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Mlo</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Container Size Type</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>Sound</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>Repaired</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>Damage</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>Wash</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>Sweep</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
+          <t>Clean</t>
+        </is>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>Total Box</t>
+        </is>
+      </c>
+      <c r="K5" s="5" t="inlineStr">
+        <is>
+          <t>Total Teus</t>
+        </is>
+      </c>
+    </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Agent</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>MLO</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>Size-Type</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>Sound</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>Repaired</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr">
-        <is>
-          <t>Damage</t>
-        </is>
-      </c>
-      <c r="G6" s="4" t="inlineStr">
-        <is>
-          <t>Wash</t>
-        </is>
-      </c>
-      <c r="H6" s="4" t="inlineStr">
-        <is>
-          <t>Sweep</t>
-        </is>
-      </c>
-      <c r="I6" s="4" t="inlineStr">
-        <is>
-          <t>Clean</t>
-        </is>
-      </c>
-      <c r="J6" s="4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="0" t="n">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -562,44 +507,42 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="75.25617977528091" hidden="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.8561797752809" hidden="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="20.713483146067418"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.213483146067416"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.213483146067418"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.213483146067418"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.213483146067418"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.713483146067418"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="10.213483146067416"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.213483146067418"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.713483146067418"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="25.213483146067418"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="21.789887640449443"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="28.213483146067418"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="17.713483146067418"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="20.713483146067418"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="25.213483146067418"/>
     <col min="17" max="17" bestFit="true" customWidth="true" width="14.713483146067416"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="16.213483146067418"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="23.713483146067418"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.713483146067416"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="11.713483146067416"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="16.213483146067418"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="22.213483146067418"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="14.713483146067416"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="14.713483146067416"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="14.713483146067416"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="5.713483146067416"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="8.713483146067416"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="10.213483146067416"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="19.213483146067418"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="8.713483146067416"/>
   </cols>
   <sheetData>
     <row ht="20" customHeight="true" r="1">
@@ -609,232 +552,215 @@
         </is>
       </c>
     </row>
-    <row ht="18" customHeight="true" r="2">
+    <row ht="16" customHeight="true" r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t> KATGHAR, NORTH PATENGA, CHITTAGONG-4204. </t>
-        </is>
-      </c>
-    </row>
-    <row ht="16" customHeight="true" r="3">
+          <t>ICB</t>
+        </is>
+      </c>
+    </row>
+    <row ht="14" customHeight="true" r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>ICB</t>
-        </is>
-      </c>
-    </row>
-    <row ht="14" customHeight="true" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
           <t>Out Empty Report</t>
         </is>
       </c>
     </row>
-    <row ht="16" customHeight="true" r="5">
-      <c r="A5" s="4" t="inlineStr">
+    <row ht="16" customHeight="true" r="4">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Total number of conatiners:1</t>
         </is>
       </c>
     </row>
-    <row r="6"/>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Container Number</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Container Size</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>Container Type</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>Current Depot Unit</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>Permitted Depot Unit</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>Mlo</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>Source Location</t>
+        </is>
+      </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>Import Vessel Name</t>
+        </is>
+      </c>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>Import Rotation Number</t>
+        </is>
+      </c>
+      <c r="L6" s="5" t="inlineStr">
+        <is>
+          <t>Gate In Date</t>
+        </is>
+      </c>
+      <c r="M6" s="5" t="inlineStr">
+        <is>
+          <t>Container Condition Name</t>
+        </is>
+      </c>
+      <c r="N6" s="5" t="inlineStr">
+        <is>
+          <t>Destination Location</t>
+        </is>
+      </c>
+      <c r="O6" s="5" t="inlineStr">
+        <is>
+          <t>Export Vessel Name</t>
+        </is>
+      </c>
+      <c r="P6" s="5" t="inlineStr">
+        <is>
+          <t>Export Rotation Number</t>
+        </is>
+      </c>
+      <c r="Q6" s="5" t="inlineStr">
+        <is>
+          <t>Stuffing Date</t>
+        </is>
+      </c>
+      <c r="R6" s="5" t="inlineStr">
+        <is>
+          <t>Gate Out Date</t>
+        </is>
+      </c>
+      <c r="S6" s="5" t="inlineStr">
+        <is>
+          <t>Eir Number</t>
+        </is>
+      </c>
+      <c r="T6" s="5" t="inlineStr">
+        <is>
+          <t>Seal No</t>
+        </is>
+      </c>
+      <c r="U6" s="5" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="V6" s="5" t="inlineStr">
+        <is>
+          <t>Vat</t>
+        </is>
+      </c>
+      <c r="W6" s="5" t="inlineStr">
+        <is>
+          <t>Cbm</t>
+        </is>
+      </c>
+      <c r="X6" s="5" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="Y6" s="5" t="inlineStr">
+        <is>
+          <t>Account</t>
+        </is>
+      </c>
+      <c r="Z6" s="5" t="inlineStr">
+        <is>
+          <t>Forwarder</t>
+        </is>
+      </c>
+      <c r="AA6" s="5" t="inlineStr">
+        <is>
+          <t>Di Agent</t>
+        </is>
+      </c>
+      <c r="AB6" s="5" t="inlineStr">
+        <is>
+          <t>Di Mlo</t>
+        </is>
+      </c>
+      <c r="AC6" s="5" t="inlineStr">
+        <is>
+          <t>Di Date</t>
+        </is>
+      </c>
+      <c r="AD6" s="5" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+    </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Container Number</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>Height</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>Company</t>
-        </is>
-      </c>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>Agent</t>
-        </is>
-      </c>
-      <c r="H7" s="4" t="inlineStr">
-        <is>
-          <t>MLO</t>
-        </is>
-      </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>Vessel</t>
-        </is>
-      </c>
-      <c r="J7" s="4" t="inlineStr">
-        <is>
-          <t>Rotation #</t>
-        </is>
-      </c>
-      <c r="K7" s="4" t="inlineStr">
-        <is>
-          <t>BE #</t>
-        </is>
-      </c>
-      <c r="L7" s="4" t="inlineStr">
-        <is>
-          <t>BL #</t>
-        </is>
-      </c>
-      <c r="M7" s="4" t="inlineStr">
-        <is>
-          <t>Line #</t>
-        </is>
-      </c>
-      <c r="N7" s="4" t="inlineStr">
-        <is>
-          <t>Importer</t>
-        </is>
-      </c>
-      <c r="O7" s="4" t="inlineStr">
-        <is>
-          <t>CNF</t>
-        </is>
-      </c>
-      <c r="P7" s="4" t="inlineStr">
-        <is>
-          <t>EIR #</t>
-        </is>
-      </c>
-      <c r="Q7" s="4" t="inlineStr">
-        <is>
-          <t>Commodity</t>
-        </is>
-      </c>
-      <c r="R7" s="4" t="inlineStr">
-        <is>
-          <t>Seal Number</t>
-        </is>
-      </c>
-      <c r="S7" s="4" t="inlineStr">
-        <is>
-          <t>Amended Seal No</t>
-        </is>
-      </c>
-      <c r="T7" s="4" t="inlineStr">
-        <is>
-          <t>Location - From</t>
-        </is>
-      </c>
-      <c r="U7" s="4" t="inlineStr">
-        <is>
-          <t>Depo Loc</t>
-        </is>
-      </c>
-      <c r="V7" s="4" t="inlineStr">
-        <is>
-          <t>Issue Date</t>
-        </is>
-      </c>
-      <c r="W7" s="4" t="inlineStr">
-        <is>
-          <t>In Date</t>
-        </is>
-      </c>
-      <c r="X7" s="4" t="inlineStr">
-        <is>
-          <t>Unstuffing Date</t>
-        </is>
-      </c>
-      <c r="Y7" s="4" t="inlineStr">
-        <is>
-          <t>Container Condition</t>
-        </is>
-      </c>
-      <c r="Z7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Area</t>
-        </is>
-      </c>
-      <c r="AA7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Part</t>
-        </is>
-      </c>
-      <c r="AB7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Description</t>
-        </is>
-      </c>
-      <c r="AC7" s="4" t="inlineStr">
-        <is>
-          <t>In Transport</t>
-        </is>
-      </c>
-      <c r="AD7" s="4" t="inlineStr">
-        <is>
-          <t>In Trailer</t>
-        </is>
-      </c>
-      <c r="AE7" s="4" t="inlineStr">
-        <is>
-          <t>Trailer #</t>
-        </is>
-      </c>
-      <c r="AF7" s="4" t="inlineStr">
-        <is>
-          <t>In Remarks</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0"/>
-      <c r="H8" s="0"/>
-      <c r="I8" s="0"/>
-      <c r="J8" s="0"/>
-      <c r="K8" s="0"/>
-      <c r="L8" s="0" t="d">
+      <c r="A7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0" t="d">
         <v>0001-01-01T00:00:00</v>
       </c>
-      <c r="M8" s="0"/>
-      <c r="N8" s="0"/>
-      <c r="O8" s="0"/>
-      <c r="P8" s="0"/>
-      <c r="Q8" s="0"/>
-      <c r="R8" s="0"/>
-      <c r="S8" s="0"/>
-      <c r="T8" s="0"/>
-      <c r="U8" s="0"/>
-      <c r="V8" s="0"/>
-      <c r="W8" s="0"/>
-      <c r="X8" s="0"/>
-      <c r="Y8" s="0"/>
-      <c r="Z8" s="0"/>
-      <c r="AA8" s="0"/>
-      <c r="AB8" s="0"/>
-      <c r="AC8" s="0"/>
-      <c r="AD8" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
@@ -857,23 +783,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="75.25617977528091" hidden="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.8561797752809" hidden="false"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.213483146067416"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.713483146067418"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="10.213483146067416"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="7.213483146067416"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.213483146067416"/>
   </cols>
   <sheetData>
     <row ht="20" customHeight="true" r="1">
@@ -883,106 +809,104 @@
         </is>
       </c>
     </row>
-    <row ht="18" customHeight="true" r="2">
+    <row ht="16" customHeight="true" r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t> KATGHAR, NORTH PATENGA, CHITTAGONG-4204. </t>
-        </is>
-      </c>
-    </row>
-    <row ht="16" customHeight="true" r="3">
+          <t>ICB</t>
+        </is>
+      </c>
+    </row>
+    <row ht="14" customHeight="true" r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>ICB</t>
-        </is>
-      </c>
-    </row>
-    <row ht="14" customHeight="true" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
           <t>Out Empty Report Summary</t>
         </is>
       </c>
     </row>
-    <row r="5"/>
+    <row r="4"/>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Mlo</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Container Size Type</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>Sound</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>Repaired</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>Damage</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>Wash</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>Sweep</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
+          <t>Clean</t>
+        </is>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>Total Box</t>
+        </is>
+      </c>
+      <c r="K5" s="5" t="inlineStr">
+        <is>
+          <t>Total Teus</t>
+        </is>
+      </c>
+    </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Agent</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>MLO</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>Size-Type</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>Sound</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>Repaired</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr">
-        <is>
-          <t>Damage</t>
-        </is>
-      </c>
-      <c r="G6" s="4" t="inlineStr">
-        <is>
-          <t>Wash</t>
-        </is>
-      </c>
-      <c r="H6" s="4" t="inlineStr">
-        <is>
-          <t>Sweep</t>
-        </is>
-      </c>
-      <c r="I6" s="4" t="inlineStr">
-        <is>
-          <t>Clean</t>
-        </is>
-      </c>
-      <c r="J6" s="4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="0" t="n">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1007,44 +931,42 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="75.25617977528091" hidden="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.8561797752809" hidden="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="20.713483146067418"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.713483146067418"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.213483146067418"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.213483146067418"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.213483146067418"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.713483146067418"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.213483146067416"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.213483146067418"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.713483146067418"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="25.213483146067418"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="21.789887640449443"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.213483146067418"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.713483146067418"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="28.213483146067418"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="17.713483146067418"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="20.713483146067418"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="25.213483146067418"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="14.713483146067416"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="16.213483146067418"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="14.713483146067416"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="11.713483146067416"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.713483146067416"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="22.213483146067418"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="14.713483146067416"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="14.713483146067416"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="5.713483146067416"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="8.713483146067416"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="10.213483146067416"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="19.213483146067418"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="10.213483146067416"/>
     <col min="29" max="29" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="14.713483146067416"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="14.713483146067416"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="13.213483146067416"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="8.713483146067416"/>
   </cols>
   <sheetData>
     <row ht="20" customHeight="true" r="1">
@@ -1054,232 +976,215 @@
         </is>
       </c>
     </row>
-    <row ht="18" customHeight="true" r="2">
+    <row ht="16" customHeight="true" r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t> KATGHAR, NORTH PATENGA, CHITTAGONG-4204. </t>
-        </is>
-      </c>
-    </row>
-    <row ht="16" customHeight="true" r="3">
+          <t>ICB</t>
+        </is>
+      </c>
+    </row>
+    <row ht="14" customHeight="true" r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>ICB</t>
-        </is>
-      </c>
-    </row>
-    <row ht="14" customHeight="true" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
           <t>Out Laden Report</t>
         </is>
       </c>
     </row>
-    <row ht="16" customHeight="true" r="5">
-      <c r="A5" s="4" t="inlineStr">
+    <row ht="16" customHeight="true" r="4">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Total number of conatiners:1</t>
         </is>
       </c>
     </row>
-    <row r="6"/>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Container Number</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Container Size</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>Container Type</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>Current Depot Unit</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>Permitted Depot Unit</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>Mlo</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>Source Location</t>
+        </is>
+      </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>Import Vessel Name</t>
+        </is>
+      </c>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>Import Rotation Number</t>
+        </is>
+      </c>
+      <c r="L6" s="5" t="inlineStr">
+        <is>
+          <t>Gate In Date</t>
+        </is>
+      </c>
+      <c r="M6" s="5" t="inlineStr">
+        <is>
+          <t>Container Condition Name</t>
+        </is>
+      </c>
+      <c r="N6" s="5" t="inlineStr">
+        <is>
+          <t>Destination Location</t>
+        </is>
+      </c>
+      <c r="O6" s="5" t="inlineStr">
+        <is>
+          <t>Export Vessel Name</t>
+        </is>
+      </c>
+      <c r="P6" s="5" t="inlineStr">
+        <is>
+          <t>Export Rotation Number</t>
+        </is>
+      </c>
+      <c r="Q6" s="5" t="inlineStr">
+        <is>
+          <t>Stuffing Date</t>
+        </is>
+      </c>
+      <c r="R6" s="5" t="inlineStr">
+        <is>
+          <t>Gate Out Date</t>
+        </is>
+      </c>
+      <c r="S6" s="5" t="inlineStr">
+        <is>
+          <t>Eir Number</t>
+        </is>
+      </c>
+      <c r="T6" s="5" t="inlineStr">
+        <is>
+          <t>Seal No</t>
+        </is>
+      </c>
+      <c r="U6" s="5" t="inlineStr">
+        <is>
+          <t>Commodity</t>
+        </is>
+      </c>
+      <c r="V6" s="5" t="inlineStr">
+        <is>
+          <t>Vat</t>
+        </is>
+      </c>
+      <c r="W6" s="5" t="inlineStr">
+        <is>
+          <t>Cbm</t>
+        </is>
+      </c>
+      <c r="X6" s="5" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="Y6" s="5" t="inlineStr">
+        <is>
+          <t>Account</t>
+        </is>
+      </c>
+      <c r="Z6" s="5" t="inlineStr">
+        <is>
+          <t>Forwarder</t>
+        </is>
+      </c>
+      <c r="AA6" s="5" t="inlineStr">
+        <is>
+          <t>Di Agent</t>
+        </is>
+      </c>
+      <c r="AB6" s="5" t="inlineStr">
+        <is>
+          <t>Di Mlo</t>
+        </is>
+      </c>
+      <c r="AC6" s="5" t="inlineStr">
+        <is>
+          <t>Di Date</t>
+        </is>
+      </c>
+      <c r="AD6" s="5" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+    </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Container Number</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>Company</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>Agent</t>
-        </is>
-      </c>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>MLO</t>
-        </is>
-      </c>
-      <c r="H7" s="4" t="inlineStr">
-        <is>
-          <t>Vessel</t>
-        </is>
-      </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>Rotation #</t>
-        </is>
-      </c>
-      <c r="J7" s="4" t="inlineStr">
-        <is>
-          <t>Importer</t>
-        </is>
-      </c>
-      <c r="K7" s="4" t="inlineStr">
-        <is>
-          <t>CNFCommodity</t>
-        </is>
-      </c>
-      <c r="L7" s="4" t="inlineStr">
-        <is>
-          <t>Current Depo</t>
-        </is>
-      </c>
-      <c r="M7" s="4" t="inlineStr">
-        <is>
-          <t>Seal Number</t>
-        </is>
-      </c>
-      <c r="N7" s="4" t="inlineStr">
-        <is>
-          <t>Amended Seal No</t>
-        </is>
-      </c>
-      <c r="O7" s="4" t="inlineStr">
-        <is>
-          <t>EIR #</t>
-        </is>
-      </c>
-      <c r="P7" s="4" t="inlineStr">
-        <is>
-          <t>BE #</t>
-        </is>
-      </c>
-      <c r="Q7" s="4" t="inlineStr">
-        <is>
-          <t>BL #</t>
-        </is>
-      </c>
-      <c r="R7" s="4" t="inlineStr">
-        <is>
-          <t>Line #</t>
-        </is>
-      </c>
-      <c r="S7" s="4" t="inlineStr">
-        <is>
-          <t>Location - From</t>
-        </is>
-      </c>
-      <c r="T7" s="4" t="inlineStr">
-        <is>
-          <t>Depo Loc</t>
-        </is>
-      </c>
-      <c r="U7" s="4" t="inlineStr">
-        <is>
-          <t>Issue Date</t>
-        </is>
-      </c>
-      <c r="V7" s="4" t="inlineStr">
-        <is>
-          <t>In Date</t>
-        </is>
-      </c>
-      <c r="W7" s="4" t="inlineStr">
-        <is>
-          <t>Out Date</t>
-        </is>
-      </c>
-      <c r="X7" s="4" t="inlineStr">
-        <is>
-          <t>Out Location</t>
-        </is>
-      </c>
-      <c r="Y7" s="4" t="inlineStr">
-        <is>
-          <t>Container Condition</t>
-        </is>
-      </c>
-      <c r="Z7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Area</t>
-        </is>
-      </c>
-      <c r="AA7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Part</t>
-        </is>
-      </c>
-      <c r="AB7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Description</t>
-        </is>
-      </c>
-      <c r="AC7" s="4" t="inlineStr">
-        <is>
-          <t>Total Lot</t>
-        </is>
-      </c>
-      <c r="AD7" s="4" t="inlineStr">
-        <is>
-          <t>Total Weight</t>
-        </is>
-      </c>
-      <c r="AE7" s="4" t="inlineStr">
-        <is>
-          <t>Out Transport</t>
-        </is>
-      </c>
-      <c r="AF7" s="4" t="inlineStr">
-        <is>
-          <t>Out Remarks</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0"/>
-      <c r="H8" s="0"/>
-      <c r="I8" s="0"/>
-      <c r="J8" s="0"/>
-      <c r="K8" s="0"/>
-      <c r="L8" s="0" t="d">
+      <c r="A7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0" t="d">
         <v>0001-01-01T00:00:00</v>
       </c>
-      <c r="M8" s="0"/>
-      <c r="N8" s="0"/>
-      <c r="O8" s="0"/>
-      <c r="P8" s="0"/>
-      <c r="Q8" s="0"/>
-      <c r="R8" s="0"/>
-      <c r="S8" s="0"/>
-      <c r="T8" s="0"/>
-      <c r="U8" s="0"/>
-      <c r="V8" s="0"/>
-      <c r="W8" s="0"/>
-      <c r="X8" s="0"/>
-      <c r="Y8" s="0"/>
-      <c r="Z8" s="0"/>
-      <c r="AA8" s="0"/>
-      <c r="AB8" s="0"/>
-      <c r="AC8" s="0"/>
-      <c r="AD8" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
@@ -1302,23 +1207,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="75.25617977528091" hidden="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.8561797752809" hidden="false"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.213483146067416"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.713483146067418"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="10.213483146067416"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="7.213483146067416"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.213483146067416"/>
   </cols>
   <sheetData>
     <row ht="20" customHeight="true" r="1">
@@ -1328,106 +1233,104 @@
         </is>
       </c>
     </row>
-    <row ht="18" customHeight="true" r="2">
+    <row ht="16" customHeight="true" r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t> KATGHAR, NORTH PATENGA, CHITTAGONG-4204. </t>
-        </is>
-      </c>
-    </row>
-    <row ht="16" customHeight="true" r="3">
+          <t>ICB</t>
+        </is>
+      </c>
+    </row>
+    <row ht="14" customHeight="true" r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>ICB</t>
-        </is>
-      </c>
-    </row>
-    <row ht="14" customHeight="true" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
           <t>Out Laden Report Summary</t>
         </is>
       </c>
     </row>
-    <row r="5"/>
+    <row r="4"/>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Mlo</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Container Size Type</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>Sound</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>Repaired</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>Damage</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>Wash</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>Sweep</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
+          <t>Clean</t>
+        </is>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>Total Box</t>
+        </is>
+      </c>
+      <c r="K5" s="5" t="inlineStr">
+        <is>
+          <t>Total Teus</t>
+        </is>
+      </c>
+    </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Agent</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>MLO</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>Size-Type</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>Sound</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>Repaired</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr">
-        <is>
-          <t>Damage</t>
-        </is>
-      </c>
-      <c r="G6" s="4" t="inlineStr">
-        <is>
-          <t>Wash</t>
-        </is>
-      </c>
-      <c r="H6" s="4" t="inlineStr">
-        <is>
-          <t>Sweep</t>
-        </is>
-      </c>
-      <c r="I6" s="4" t="inlineStr">
-        <is>
-          <t>Clean</t>
-        </is>
-      </c>
-      <c r="J6" s="4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="0" t="n">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1452,41 +1355,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:AA34"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="75.25617977528091" hidden="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.8561797752809" hidden="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="20.713483146067418"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.48988764044944"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.989887640449439"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="22.213483146067418"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.213483146067418"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.213483146067418"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.213483146067416"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.213483146067416"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.213483146067418"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.713483146067418"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.713483146067418"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="25.213483146067418"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="16.213483146067418"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="21.789887640449443"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.213483146067418"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="14.713483146067416"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.213483146067418"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="23.713483146067418"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="28.213483146067418"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.213483146067416"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.713483146067416"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.213483146067418"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.213483146067418"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="13.213483146067416"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="10.213483146067416"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="14.713483146067416"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="20.713483146067418"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="47.08988764044945"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="78.98988764044944"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.213483146067416"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.213483146067416"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.713483146067418"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="17.713483146067418"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.213483146067418"/>
   </cols>
   <sheetData>
     <row ht="20" customHeight="true" r="1">
@@ -1496,197 +1397,289 @@
         </is>
       </c>
     </row>
-    <row ht="18" customHeight="true" r="2">
+    <row ht="16" customHeight="true" r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t> KATGHAR, NORTH PATENGA, CHITTAGONG-4204. </t>
-        </is>
-      </c>
-    </row>
-    <row ht="16" customHeight="true" r="3">
+          <t>ICB</t>
+        </is>
+      </c>
+    </row>
+    <row ht="14" customHeight="true" r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
+          <t>Stock Report</t>
+        </is>
+      </c>
+    </row>
+    <row ht="16" customHeight="true" r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>Total number of conatiners:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Container Number</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Container Size</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>Container Type</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>Mlo</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>Current Depot Unit</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>Permitted Depot Unit</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>Import Vessel Name</t>
+        </is>
+      </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>Import Rotation Number</t>
+        </is>
+      </c>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>Source Location</t>
+        </is>
+      </c>
+      <c r="L6" s="4" t="inlineStr">
+        <is>
+          <t>Gate In Date</t>
+        </is>
+      </c>
+      <c r="M6" s="4" t="inlineStr">
+        <is>
+          <t>Container Condition Name</t>
+        </is>
+      </c>
+      <c r="N6" s="4" t="inlineStr">
+        <is>
+          <t>Bay Location</t>
+        </is>
+      </c>
+      <c r="O6" s="5" t="inlineStr">
+        <is>
+          <t>Storage Day</t>
+        </is>
+      </c>
+      <c r="P6" s="5" t="inlineStr">
+        <is>
+          <t>Container Status</t>
+        </is>
+      </c>
+      <c r="Q6" s="5" t="inlineStr">
+        <is>
+          <t>Container Status Name</t>
+        </is>
+      </c>
+      <c r="R6" s="5" t="inlineStr">
+        <is>
+          <t>Di Agent</t>
+        </is>
+      </c>
+      <c r="S6" s="5" t="inlineStr">
+        <is>
+          <t>Di Mlo</t>
+        </is>
+      </c>
+      <c r="T6" s="5" t="inlineStr">
+        <is>
+          <t>Di Date</t>
+        </is>
+      </c>
+      <c r="U6" s="5" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+      <c r="V6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Area Name</t>
+        </is>
+      </c>
+      <c r="W6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Part Name</t>
+        </is>
+      </c>
+      <c r="X6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Description</t>
+        </is>
+      </c>
+      <c r="Y6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Component</t>
+        </is>
+      </c>
+      <c r="Z6" s="5" t="inlineStr">
+        <is>
+          <t>Damage Type</t>
+        </is>
+      </c>
+      <c r="AA6" s="5" t="inlineStr">
+        <is>
+          <t>Repair Type</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>37003</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>FCIU8848750</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>BS</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
           <t>ICB</t>
         </is>
       </c>
-    </row>
-    <row ht="14" customHeight="true" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>Stock Report</t>
-        </is>
-      </c>
-    </row>
-    <row ht="16" customHeight="true" r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>Total number of conatiners:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="6"/>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Container Number</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>Company</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>Agent</t>
-        </is>
-      </c>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>MLO</t>
-        </is>
-      </c>
-      <c r="H7" s="4" t="inlineStr">
-        <is>
-          <t>Vessel</t>
-        </is>
-      </c>
-      <c r="I7" s="4" t="inlineStr">
-        <is>
-          <t>Rotation #</t>
-        </is>
-      </c>
-      <c r="J7" s="4" t="inlineStr">
-        <is>
-          <t>Importer</t>
-        </is>
-      </c>
-      <c r="K7" s="4" t="inlineStr">
-        <is>
-          <t>Container Condition</t>
-        </is>
-      </c>
-      <c r="L7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Area</t>
-        </is>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t>SAPL-W</t>
+        </is>
+      </c>
+      <c r="H7" s="0" t="inlineStr">
+        <is>
+          <t>SAPL-W</t>
+        </is>
+      </c>
+      <c r="I7" s="0" t="inlineStr">
+        <is>
+          <t>M.TARABA-18012</t>
+        </is>
+      </c>
+      <c r="J7" s="0" t="inlineStr">
+        <is>
+          <t>2018/1861</t>
+        </is>
+      </c>
+      <c r="K7" s="0" t="inlineStr">
+        <is>
+          <t>CPA</t>
+        </is>
+      </c>
+      <c r="L7" s="4" t="d">
+        <v>2018-06-20T00:00:00</v>
       </c>
       <c r="M7" s="4" t="inlineStr">
         <is>
-          <t>Damage Part</t>
-        </is>
-      </c>
-      <c r="N7" s="4" t="inlineStr">
-        <is>
-          <t>Damage Description</t>
-        </is>
-      </c>
-      <c r="O7" s="4" t="inlineStr">
-        <is>
-          <t>CNF</t>
-        </is>
-      </c>
-      <c r="P7" s="4" t="inlineStr">
-        <is>
-          <t>Commodity</t>
-        </is>
-      </c>
-      <c r="Q7" s="4" t="inlineStr">
-        <is>
-          <t>Seal Number</t>
-        </is>
-      </c>
-      <c r="R7" s="4" t="inlineStr">
-        <is>
-          <t>Amended Seal No</t>
-        </is>
-      </c>
-      <c r="S7" s="4" t="inlineStr">
-        <is>
-          <t>EIR #</t>
-        </is>
-      </c>
-      <c r="T7" s="4" t="inlineStr">
-        <is>
-          <t>Issue Date</t>
-        </is>
-      </c>
-      <c r="U7" s="4" t="inlineStr">
-        <is>
-          <t>In Date</t>
-        </is>
-      </c>
-      <c r="V7" s="4" t="inlineStr">
-        <is>
-          <t>Location - From</t>
-        </is>
-      </c>
-      <c r="W7" s="4" t="inlineStr">
-        <is>
-          <t>Depo Loc</t>
-        </is>
-      </c>
-      <c r="X7" s="4" t="inlineStr">
-        <is>
-          <t>BE #</t>
-        </is>
-      </c>
-      <c r="Y7" s="4" t="inlineStr">
-        <is>
-          <t>BL #</t>
-        </is>
-      </c>
-      <c r="Z7" s="4" t="inlineStr">
-        <is>
-          <t>Line #</t>
-        </is>
-      </c>
-      <c r="AA7" s="4" t="inlineStr">
-        <is>
-          <t>Trailer #</t>
-        </is>
-      </c>
-      <c r="AB7" s="4" t="inlineStr">
-        <is>
-          <t>In Transport</t>
-        </is>
-      </c>
-      <c r="AC7" s="4" t="inlineStr">
-        <is>
-          <t>In Remarks</t>
+          <t>DAMAGE</t>
+        </is>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="0" t="inlineStr">
+        <is>
+          <t>Empty</t>
+        </is>
+      </c>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0" t="n">
+        <v>1442298</v>
+      </c>
+      <c r="V7" s="0" t="inlineStr">
+        <is>
+          <t>DOORS-(D)</t>
+        </is>
+      </c>
+      <c r="W7" s="0" t="inlineStr">
+        <is>
+          <t>Door stiffeners hinges side edge.-(Door stiffeners hinges side edge.)</t>
+        </is>
+      </c>
+      <c r="X7" s="0" t="inlineStr">
+        <is>
+          <t>BOTH DOOR LOCK BAR HANDEL BENT 02 PCS.</t>
+        </is>
+      </c>
+      <c r="Y7" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Z7" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA7" s="0" t="inlineStr">
+        <is>
+          <t/>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="n">
-        <v>37442</v>
+        <v>37003</v>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>TCKU3712139</t>
+          <t>FCIU8848750</t>
         </is>
       </c>
       <c r="C8" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
@@ -1711,30 +1704,30 @@
       </c>
       <c r="I8" s="0" t="inlineStr">
         <is>
-          <t>XP. KOHIMA</t>
+          <t>M.TARABA-18012</t>
         </is>
       </c>
       <c r="J8" s="0" t="inlineStr">
         <is>
-          <t>2018/1719</t>
+          <t>2018/1861</t>
         </is>
       </c>
       <c r="K8" s="0" t="inlineStr">
         <is>
-          <t>OTC</t>
-        </is>
-      </c>
-      <c r="L8" s="0" t="d">
-        <v>2018-06-27T00:00:00</v>
-      </c>
-      <c r="M8" s="0" t="inlineStr">
-        <is>
-          <t>WASH</t>
-        </is>
-      </c>
-      <c r="N8" s="0"/>
+          <t>CPA</t>
+        </is>
+      </c>
+      <c r="L8" s="4" t="d">
+        <v>2018-06-20T00:00:00</v>
+      </c>
+      <c r="M8" s="4" t="inlineStr">
+        <is>
+          <t>DAMAGE</t>
+        </is>
+      </c>
+      <c r="N8" s="4"/>
       <c r="O8" s="0" t="n">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="P8" s="0" t="n">
         <v>0</v>
@@ -1748,21 +1741,21 @@
       <c r="S8" s="0"/>
       <c r="T8" s="0"/>
       <c r="U8" s="0" t="n">
-        <v>1471692</v>
+        <v>1442298</v>
       </c>
       <c r="V8" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W8" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X8" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>FLOOR BOARD SLIGHTLY UP WARD.</t>
         </is>
       </c>
       <c r="Y8" s="0" t="inlineStr">
@@ -1783,19 +1776,19 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="n">
-        <v>37442</v>
+        <v>37003</v>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>TCKU3712139</t>
+          <t>FCIU8848750</t>
         </is>
       </c>
       <c r="C9" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
@@ -1820,30 +1813,30 @@
       </c>
       <c r="I9" s="0" t="inlineStr">
         <is>
-          <t>XP. KOHIMA</t>
+          <t>M.TARABA-18012</t>
         </is>
       </c>
       <c r="J9" s="0" t="inlineStr">
         <is>
-          <t>2018/1719</t>
+          <t>2018/1861</t>
         </is>
       </c>
       <c r="K9" s="0" t="inlineStr">
         <is>
-          <t>OTC</t>
-        </is>
-      </c>
-      <c r="L9" s="0" t="d">
-        <v>2018-06-27T00:00:00</v>
-      </c>
-      <c r="M9" s="0" t="inlineStr">
-        <is>
-          <t>WASH</t>
-        </is>
-      </c>
-      <c r="N9" s="0"/>
+          <t>CPA</t>
+        </is>
+      </c>
+      <c r="L9" s="4" t="d">
+        <v>2018-06-20T00:00:00</v>
+      </c>
+      <c r="M9" s="4" t="inlineStr">
+        <is>
+          <t>DAMAGE</t>
+        </is>
+      </c>
+      <c r="N9" s="4"/>
       <c r="O9" s="0" t="n">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="P9" s="0" t="n">
         <v>0</v>
@@ -1857,7 +1850,7 @@
       <c r="S9" s="0"/>
       <c r="T9" s="0"/>
       <c r="U9" s="0" t="n">
-        <v>1471692</v>
+        <v>1442298</v>
       </c>
       <c r="V9" s="0" t="inlineStr">
         <is>
@@ -1866,12 +1859,12 @@
       </c>
       <c r="W9" s="0" t="inlineStr">
         <is>
-          <t>FLOOR BOARD-(FLOOR BOARD)</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X9" s="0" t="inlineStr">
         <is>
-          <t>F/BOARD DIRTY BY BADLY SCRAP DUST &amp; SCRATCHED.</t>
+          <t>FLOOR BOARD DIRTY BY DUST.</t>
         </is>
       </c>
       <c r="Y9" s="0" t="inlineStr">
@@ -1892,19 +1885,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="n">
-        <v>39412</v>
+        <v>37040</v>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>CAIU9708712</t>
+          <t>IAAU2753116</t>
         </is>
       </c>
       <c r="C10" s="0" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>GP</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
@@ -1919,7 +1912,7 @@
       </c>
       <c r="G10" s="0" t="inlineStr">
         <is>
-          <t>SAPL-W</t>
+          <t>SAPL-E</t>
         </is>
       </c>
       <c r="H10" s="0" t="inlineStr">
@@ -1929,30 +1922,30 @@
       </c>
       <c r="I10" s="0" t="inlineStr">
         <is>
-          <t>XPRESS LHOTSE</t>
+          <t>MV.X-PRESS KOHIMA</t>
         </is>
       </c>
       <c r="J10" s="0" t="inlineStr">
         <is>
-          <t>2703/2018</t>
+          <t>2018/1935</t>
         </is>
       </c>
       <c r="K10" s="0" t="inlineStr">
         <is>
-          <t>IMPORT</t>
-        </is>
-      </c>
-      <c r="L10" s="0" t="d">
-        <v>2018-09-15T00:00:00</v>
-      </c>
-      <c r="M10" s="0" t="inlineStr">
-        <is>
-          <t>WASH</t>
-        </is>
-      </c>
-      <c r="N10" s="0"/>
+          <t>OTC</t>
+        </is>
+      </c>
+      <c r="L10" s="4" t="d">
+        <v>2018-07-03T00:00:00</v>
+      </c>
+      <c r="M10" s="4" t="inlineStr">
+        <is>
+          <t>CLEANED</t>
+        </is>
+      </c>
+      <c r="N10" s="4"/>
       <c r="O10" s="0" t="n">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="P10" s="0" t="n">
         <v>0</v>
@@ -1966,7 +1959,7 @@
       <c r="S10" s="0"/>
       <c r="T10" s="0"/>
       <c r="U10" s="0" t="n">
-        <v>1479843</v>
+        <v>1447518</v>
       </c>
       <c r="V10" s="0" t="inlineStr">
         <is>
@@ -1980,7 +1973,7 @@
       </c>
       <c r="X10" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY DROP OIL SPOT,TYER MARK, &amp; BADLY MUD DUST.</t>
+          <t>FLOOR BOARD DIRTY BY DUST.</t>
         </is>
       </c>
       <c r="Y10" s="0" t="inlineStr">
@@ -2001,19 +1994,19 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="n">
-        <v>39413</v>
+        <v>37442</v>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>IAAU1727576</t>
+          <t>TCKU3712139</t>
         </is>
       </c>
       <c r="C11" s="0" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>GP</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
@@ -2033,35 +2026,35 @@
       </c>
       <c r="H11" s="0" t="inlineStr">
         <is>
-          <t>SAPL-E</t>
+          <t>SAPL-W</t>
         </is>
       </c>
       <c r="I11" s="0" t="inlineStr">
         <is>
-          <t>XPRESS LHOTSE</t>
+          <t>XP. KOHIMA</t>
         </is>
       </c>
       <c r="J11" s="0" t="inlineStr">
         <is>
-          <t>2703/2018</t>
+          <t>2018/1719</t>
         </is>
       </c>
       <c r="K11" s="0" t="inlineStr">
         <is>
-          <t>IMPORT</t>
-        </is>
-      </c>
-      <c r="L11" s="0" t="d">
-        <v>2018-09-15T00:00:00</v>
-      </c>
-      <c r="M11" s="0" t="inlineStr">
+          <t>OTC</t>
+        </is>
+      </c>
+      <c r="L11" s="4" t="d">
+        <v>2018-06-27T00:00:00</v>
+      </c>
+      <c r="M11" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N11" s="0"/>
+      <c r="N11" s="4"/>
       <c r="O11" s="0" t="n">
-        <v>74</v>
+        <v>154</v>
       </c>
       <c r="P11" s="0" t="n">
         <v>0</v>
@@ -2075,21 +2068,21 @@
       <c r="S11" s="0"/>
       <c r="T11" s="0"/>
       <c r="U11" s="0" t="n">
-        <v>1479844</v>
+        <v>1471692</v>
       </c>
       <c r="V11" s="0" t="inlineStr">
         <is>
-          <t>FLOORS-(F)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W11" s="0" t="inlineStr">
         <is>
-          <t>Threshold plate-(Threshold plate)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X11" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY DROP OIL SPOT,TYER MARK, &amp; BADLY MUD DUST.</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y11" s="0" t="inlineStr">
@@ -2110,19 +2103,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="n">
-        <v>39414</v>
+        <v>37442</v>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>IAAU1743330</t>
+          <t>TCKU3712139</t>
         </is>
       </c>
       <c r="C12" s="0" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>HC</t>
+          <t>GP</t>
         </is>
       </c>
       <c r="E12" s="0" t="inlineStr">
@@ -2142,35 +2135,35 @@
       </c>
       <c r="H12" s="0" t="inlineStr">
         <is>
-          <t>SAPL-E</t>
+          <t>SAPL-W</t>
         </is>
       </c>
       <c r="I12" s="0" t="inlineStr">
         <is>
-          <t>XPRESS LHOTSE</t>
+          <t>XP. KOHIMA</t>
         </is>
       </c>
       <c r="J12" s="0" t="inlineStr">
         <is>
-          <t>2703/2018</t>
+          <t>2018/1719</t>
         </is>
       </c>
       <c r="K12" s="0" t="inlineStr">
         <is>
-          <t>IMPORT</t>
-        </is>
-      </c>
-      <c r="L12" s="0" t="d">
-        <v>2018-09-15T00:00:00</v>
-      </c>
-      <c r="M12" s="0" t="inlineStr">
+          <t>OTC</t>
+        </is>
+      </c>
+      <c r="L12" s="4" t="d">
+        <v>2018-06-27T00:00:00</v>
+      </c>
+      <c r="M12" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N12" s="0"/>
+      <c r="N12" s="4"/>
       <c r="O12" s="0" t="n">
-        <v>74</v>
+        <v>154</v>
       </c>
       <c r="P12" s="0" t="n">
         <v>0</v>
@@ -2184,21 +2177,21 @@
       <c r="S12" s="0"/>
       <c r="T12" s="0"/>
       <c r="U12" s="0" t="n">
-        <v>1479846</v>
+        <v>1471692</v>
       </c>
       <c r="V12" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W12" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>FLOOR BOARD-(FLOOR BOARD)</t>
         </is>
       </c>
       <c r="X12" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>F/BOARD DIRTY BY BADLY SCRAP DUST &amp; SCRATCHED.</t>
         </is>
       </c>
       <c r="Y12" s="0" t="inlineStr">
@@ -2219,11 +2212,11 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="n">
-        <v>39414</v>
+        <v>39412</v>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>IAAU1743330</t>
+          <t>CAIU9708712</t>
         </is>
       </c>
       <c r="C13" s="0" t="n">
@@ -2269,15 +2262,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L13" s="0" t="d">
+      <c r="L13" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M13" s="0" t="inlineStr">
+      <c r="M13" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N13" s="0"/>
+      <c r="N13" s="4"/>
       <c r="O13" s="0" t="n">
         <v>74</v>
       </c>
@@ -2293,7 +2286,7 @@
       <c r="S13" s="0"/>
       <c r="T13" s="0"/>
       <c r="U13" s="0" t="n">
-        <v>1479846</v>
+        <v>1479843</v>
       </c>
       <c r="V13" s="0" t="inlineStr">
         <is>
@@ -2307,7 +2300,7 @@
       </c>
       <c r="X13" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST &amp; ODOUR </t>
+          <t>F/B DIRTY BY DROP OIL SPOT,TYER MARK, &amp; BADLY MUD DUST.</t>
         </is>
       </c>
       <c r="Y13" s="0" t="inlineStr">
@@ -2328,11 +2321,11 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="n">
-        <v>39415</v>
+        <v>39413</v>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>IAAU1702860</t>
+          <t>IAAU1727576</t>
         </is>
       </c>
       <c r="C14" s="0" t="n">
@@ -2378,15 +2371,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L14" s="0" t="d">
+      <c r="L14" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M14" s="0" t="inlineStr">
+      <c r="M14" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N14" s="0"/>
+      <c r="N14" s="4"/>
       <c r="O14" s="0" t="n">
         <v>74</v>
       </c>
@@ -2402,21 +2395,21 @@
       <c r="S14" s="0"/>
       <c r="T14" s="0"/>
       <c r="U14" s="0" t="n">
-        <v>1479848</v>
+        <v>1479844</v>
       </c>
       <c r="V14" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W14" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X14" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>F/B DIRTY BY DROP OIL SPOT,TYER MARK, &amp; BADLY MUD DUST.</t>
         </is>
       </c>
       <c r="Y14" s="0" t="inlineStr">
@@ -2437,11 +2430,11 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="n">
-        <v>39415</v>
+        <v>39414</v>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>IAAU1702860</t>
+          <t>IAAU1743330</t>
         </is>
       </c>
       <c r="C15" s="0" t="n">
@@ -2487,15 +2480,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L15" s="0" t="d">
+      <c r="L15" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M15" s="0" t="inlineStr">
+      <c r="M15" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N15" s="0"/>
+      <c r="N15" s="4"/>
       <c r="O15" s="0" t="n">
         <v>74</v>
       </c>
@@ -2511,21 +2504,21 @@
       <c r="S15" s="0"/>
       <c r="T15" s="0"/>
       <c r="U15" s="0" t="n">
-        <v>1479848</v>
+        <v>1479846</v>
       </c>
       <c r="V15" s="0" t="inlineStr">
         <is>
-          <t>FLOORS-(F)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W15" s="0" t="inlineStr">
         <is>
-          <t>Threshold plate-(Threshold plate)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X15" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y15" s="0" t="inlineStr">
@@ -2546,11 +2539,11 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="n">
-        <v>39416</v>
+        <v>39414</v>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>CAIU9708266</t>
+          <t>IAAU1743330</t>
         </is>
       </c>
       <c r="C16" s="0" t="n">
@@ -2596,15 +2589,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L16" s="0" t="d">
+      <c r="L16" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M16" s="0" t="inlineStr">
+      <c r="M16" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N16" s="0"/>
+      <c r="N16" s="4"/>
       <c r="O16" s="0" t="n">
         <v>74</v>
       </c>
@@ -2620,21 +2613,21 @@
       <c r="S16" s="0"/>
       <c r="T16" s="0"/>
       <c r="U16" s="0" t="n">
-        <v>1479849</v>
+        <v>1479846</v>
       </c>
       <c r="V16" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W16" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X16" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST &amp; ODOUR </t>
         </is>
       </c>
       <c r="Y16" s="0" t="inlineStr">
@@ -2655,11 +2648,11 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="n">
-        <v>39416</v>
+        <v>39415</v>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>CAIU9708266</t>
+          <t>IAAU1702860</t>
         </is>
       </c>
       <c r="C17" s="0" t="n">
@@ -2705,15 +2698,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L17" s="0" t="d">
+      <c r="L17" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M17" s="0" t="inlineStr">
+      <c r="M17" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N17" s="0"/>
+      <c r="N17" s="4"/>
       <c r="O17" s="0" t="n">
         <v>74</v>
       </c>
@@ -2729,21 +2722,21 @@
       <c r="S17" s="0"/>
       <c r="T17" s="0"/>
       <c r="U17" s="0" t="n">
-        <v>1479849</v>
+        <v>1479848</v>
       </c>
       <c r="V17" s="0" t="inlineStr">
         <is>
-          <t>FLOORS-(F)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W17" s="0" t="inlineStr">
         <is>
-          <t>Threshold plate-(Threshold plate)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X17" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y17" s="0" t="inlineStr">
@@ -2764,11 +2757,11 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="n">
-        <v>39417</v>
+        <v>39415</v>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>TCNU9004548</t>
+          <t>IAAU1702860</t>
         </is>
       </c>
       <c r="C18" s="0" t="n">
@@ -2814,15 +2807,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L18" s="0" t="d">
+      <c r="L18" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M18" s="0" t="inlineStr">
+      <c r="M18" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N18" s="0"/>
+      <c r="N18" s="4"/>
       <c r="O18" s="0" t="n">
         <v>74</v>
       </c>
@@ -2838,21 +2831,21 @@
       <c r="S18" s="0"/>
       <c r="T18" s="0"/>
       <c r="U18" s="0" t="n">
-        <v>1479850</v>
+        <v>1479848</v>
       </c>
       <c r="V18" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W18" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X18" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
         </is>
       </c>
       <c r="Y18" s="0" t="inlineStr">
@@ -2873,11 +2866,11 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="n">
-        <v>39417</v>
+        <v>39416</v>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>TCNU9004548</t>
+          <t>CAIU9708266</t>
         </is>
       </c>
       <c r="C19" s="0" t="n">
@@ -2923,15 +2916,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L19" s="0" t="d">
+      <c r="L19" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M19" s="0" t="inlineStr">
+      <c r="M19" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N19" s="0"/>
+      <c r="N19" s="4"/>
       <c r="O19" s="0" t="n">
         <v>74</v>
       </c>
@@ -2947,21 +2940,21 @@
       <c r="S19" s="0"/>
       <c r="T19" s="0"/>
       <c r="U19" s="0" t="n">
-        <v>1479850</v>
+        <v>1479849</v>
       </c>
       <c r="V19" s="0" t="inlineStr">
         <is>
-          <t>FLOORS-(F)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W19" s="0" t="inlineStr">
         <is>
-          <t>Threshold plate-(Threshold plate)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X19" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y19" s="0" t="inlineStr">
@@ -2982,11 +2975,11 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="n">
-        <v>39418</v>
+        <v>39416</v>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>IAAU1683210</t>
+          <t>CAIU9708266</t>
         </is>
       </c>
       <c r="C20" s="0" t="n">
@@ -3032,15 +3025,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L20" s="0" t="d">
+      <c r="L20" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M20" s="0" t="inlineStr">
+      <c r="M20" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N20" s="0"/>
+      <c r="N20" s="4"/>
       <c r="O20" s="0" t="n">
         <v>74</v>
       </c>
@@ -3056,21 +3049,21 @@
       <c r="S20" s="0"/>
       <c r="T20" s="0"/>
       <c r="U20" s="0" t="n">
-        <v>1479852</v>
+        <v>1479849</v>
       </c>
       <c r="V20" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W20" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X20" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
         </is>
       </c>
       <c r="Y20" s="0" t="inlineStr">
@@ -3091,11 +3084,11 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="n">
-        <v>39418</v>
+        <v>39417</v>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>IAAU1683210</t>
+          <t>TCNU9004548</t>
         </is>
       </c>
       <c r="C21" s="0" t="n">
@@ -3141,15 +3134,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L21" s="0" t="d">
+      <c r="L21" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M21" s="0" t="inlineStr">
+      <c r="M21" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N21" s="0"/>
+      <c r="N21" s="4"/>
       <c r="O21" s="0" t="n">
         <v>74</v>
       </c>
@@ -3165,21 +3158,21 @@
       <c r="S21" s="0"/>
       <c r="T21" s="0"/>
       <c r="U21" s="0" t="n">
-        <v>1479852</v>
+        <v>1479850</v>
       </c>
       <c r="V21" s="0" t="inlineStr">
         <is>
-          <t>FLOORS-(F)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W21" s="0" t="inlineStr">
         <is>
-          <t>Threshold plate-(Threshold plate)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X21" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y21" s="0" t="inlineStr">
@@ -3200,11 +3193,11 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="n">
-        <v>39419</v>
+        <v>39417</v>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>IAAU1732150</t>
+          <t>TCNU9004548</t>
         </is>
       </c>
       <c r="C22" s="0" t="n">
@@ -3250,15 +3243,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L22" s="0" t="d">
+      <c r="L22" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M22" s="0" t="inlineStr">
+      <c r="M22" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N22" s="0"/>
+      <c r="N22" s="4"/>
       <c r="O22" s="0" t="n">
         <v>74</v>
       </c>
@@ -3274,21 +3267,21 @@
       <c r="S22" s="0"/>
       <c r="T22" s="0"/>
       <c r="U22" s="0" t="n">
-        <v>1479853</v>
+        <v>1479850</v>
       </c>
       <c r="V22" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W22" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X22" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
         </is>
       </c>
       <c r="Y22" s="0" t="inlineStr">
@@ -3309,11 +3302,11 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="n">
-        <v>39419</v>
+        <v>39418</v>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>IAAU1732150</t>
+          <t>IAAU1683210</t>
         </is>
       </c>
       <c r="C23" s="0" t="n">
@@ -3359,15 +3352,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L23" s="0" t="d">
+      <c r="L23" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M23" s="0" t="inlineStr">
+      <c r="M23" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N23" s="0"/>
+      <c r="N23" s="4"/>
       <c r="O23" s="0" t="n">
         <v>74</v>
       </c>
@@ -3383,21 +3376,21 @@
       <c r="S23" s="0"/>
       <c r="T23" s="0"/>
       <c r="U23" s="0" t="n">
-        <v>1479853</v>
+        <v>1479852</v>
       </c>
       <c r="V23" s="0" t="inlineStr">
         <is>
-          <t>FLOORS-(F)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W23" s="0" t="inlineStr">
         <is>
-          <t>Threshold plate-(Threshold plate)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X23" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y23" s="0" t="inlineStr">
@@ -3418,11 +3411,11 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="n">
-        <v>39420</v>
+        <v>39418</v>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>IAAU1695967</t>
+          <t>IAAU1683210</t>
         </is>
       </c>
       <c r="C24" s="0" t="n">
@@ -3468,15 +3461,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L24" s="0" t="d">
+      <c r="L24" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M24" s="0" t="inlineStr">
+      <c r="M24" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N24" s="0"/>
+      <c r="N24" s="4"/>
       <c r="O24" s="0" t="n">
         <v>74</v>
       </c>
@@ -3492,7 +3485,7 @@
       <c r="S24" s="0"/>
       <c r="T24" s="0"/>
       <c r="U24" s="0" t="n">
-        <v>1479854</v>
+        <v>1479852</v>
       </c>
       <c r="V24" s="0" t="inlineStr">
         <is>
@@ -3506,7 +3499,7 @@
       </c>
       <c r="X24" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY DROP OIL SPOT,TYER MARK, &amp; BADLY MUD DUST.</t>
+          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
         </is>
       </c>
       <c r="Y24" s="0" t="inlineStr">
@@ -3527,11 +3520,11 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="n">
-        <v>37003</v>
+        <v>39419</v>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>FCIU8848750</t>
+          <t>IAAU1732150</t>
         </is>
       </c>
       <c r="C25" s="0" t="n">
@@ -3559,35 +3552,35 @@
       </c>
       <c r="H25" s="0" t="inlineStr">
         <is>
-          <t>SAPL-W</t>
+          <t>SAPL-E</t>
         </is>
       </c>
       <c r="I25" s="0" t="inlineStr">
         <is>
-          <t>M.TARABA-18012</t>
+          <t>XPRESS LHOTSE</t>
         </is>
       </c>
       <c r="J25" s="0" t="inlineStr">
         <is>
-          <t>2018/1861</t>
+          <t>2703/2018</t>
         </is>
       </c>
       <c r="K25" s="0" t="inlineStr">
         <is>
-          <t>CPA</t>
-        </is>
-      </c>
-      <c r="L25" s="0" t="d">
-        <v>2018-06-20T00:00:00</v>
-      </c>
-      <c r="M25" s="0" t="inlineStr">
-        <is>
-          <t>DAMAGE</t>
-        </is>
-      </c>
-      <c r="N25" s="0"/>
+          <t>IMPORT</t>
+        </is>
+      </c>
+      <c r="L25" s="4" t="d">
+        <v>2018-09-15T00:00:00</v>
+      </c>
+      <c r="M25" s="4" t="inlineStr">
+        <is>
+          <t>WASH</t>
+        </is>
+      </c>
+      <c r="N25" s="4"/>
       <c r="O25" s="0" t="n">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="P25" s="0" t="n">
         <v>0</v>
@@ -3601,21 +3594,21 @@
       <c r="S25" s="0"/>
       <c r="T25" s="0"/>
       <c r="U25" s="0" t="n">
-        <v>1442298</v>
+        <v>1479853</v>
       </c>
       <c r="V25" s="0" t="inlineStr">
         <is>
-          <t>DOORS-(D)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W25" s="0" t="inlineStr">
         <is>
-          <t>Door stiffeners hinges side edge.-(Door stiffeners hinges side edge.)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X25" s="0" t="inlineStr">
         <is>
-          <t>BOTH DOOR LOCK BAR HANDEL BENT 02 PCS.</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y25" s="0" t="inlineStr">
@@ -3636,11 +3629,11 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="n">
-        <v>37003</v>
+        <v>39419</v>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>FCIU8848750</t>
+          <t>IAAU1732150</t>
         </is>
       </c>
       <c r="C26" s="0" t="n">
@@ -3668,35 +3661,35 @@
       </c>
       <c r="H26" s="0" t="inlineStr">
         <is>
-          <t>SAPL-W</t>
+          <t>SAPL-E</t>
         </is>
       </c>
       <c r="I26" s="0" t="inlineStr">
         <is>
-          <t>M.TARABA-18012</t>
+          <t>XPRESS LHOTSE</t>
         </is>
       </c>
       <c r="J26" s="0" t="inlineStr">
         <is>
-          <t>2018/1861</t>
+          <t>2703/2018</t>
         </is>
       </c>
       <c r="K26" s="0" t="inlineStr">
         <is>
-          <t>CPA</t>
-        </is>
-      </c>
-      <c r="L26" s="0" t="d">
-        <v>2018-06-20T00:00:00</v>
-      </c>
-      <c r="M26" s="0" t="inlineStr">
-        <is>
-          <t>DAMAGE</t>
-        </is>
-      </c>
-      <c r="N26" s="0"/>
+          <t>IMPORT</t>
+        </is>
+      </c>
+      <c r="L26" s="4" t="d">
+        <v>2018-09-15T00:00:00</v>
+      </c>
+      <c r="M26" s="4" t="inlineStr">
+        <is>
+          <t>WASH</t>
+        </is>
+      </c>
+      <c r="N26" s="4"/>
       <c r="O26" s="0" t="n">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="P26" s="0" t="n">
         <v>0</v>
@@ -3710,7 +3703,7 @@
       <c r="S26" s="0"/>
       <c r="T26" s="0"/>
       <c r="U26" s="0" t="n">
-        <v>1442298</v>
+        <v>1479853</v>
       </c>
       <c r="V26" s="0" t="inlineStr">
         <is>
@@ -3724,7 +3717,7 @@
       </c>
       <c r="X26" s="0" t="inlineStr">
         <is>
-          <t>FLOOR BOARD SLIGHTLY UP WARD.</t>
+          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
         </is>
       </c>
       <c r="Y26" s="0" t="inlineStr">
@@ -3745,11 +3738,11 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="n">
-        <v>37003</v>
+        <v>39420</v>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>FCIU8848750</t>
+          <t>IAAU1695967</t>
         </is>
       </c>
       <c r="C27" s="0" t="n">
@@ -3777,35 +3770,35 @@
       </c>
       <c r="H27" s="0" t="inlineStr">
         <is>
-          <t>SAPL-W</t>
+          <t>SAPL-E</t>
         </is>
       </c>
       <c r="I27" s="0" t="inlineStr">
         <is>
-          <t>M.TARABA-18012</t>
+          <t>XPRESS LHOTSE</t>
         </is>
       </c>
       <c r="J27" s="0" t="inlineStr">
         <is>
-          <t>2018/1861</t>
+          <t>2703/2018</t>
         </is>
       </c>
       <c r="K27" s="0" t="inlineStr">
         <is>
-          <t>CPA</t>
-        </is>
-      </c>
-      <c r="L27" s="0" t="d">
-        <v>2018-06-20T00:00:00</v>
-      </c>
-      <c r="M27" s="0" t="inlineStr">
-        <is>
-          <t>DAMAGE</t>
-        </is>
-      </c>
-      <c r="N27" s="0"/>
+          <t>IMPORT</t>
+        </is>
+      </c>
+      <c r="L27" s="4" t="d">
+        <v>2018-09-15T00:00:00</v>
+      </c>
+      <c r="M27" s="4" t="inlineStr">
+        <is>
+          <t>WASH</t>
+        </is>
+      </c>
+      <c r="N27" s="4"/>
       <c r="O27" s="0" t="n">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="P27" s="0" t="n">
         <v>0</v>
@@ -3819,7 +3812,7 @@
       <c r="S27" s="0"/>
       <c r="T27" s="0"/>
       <c r="U27" s="0" t="n">
-        <v>1442298</v>
+        <v>1479854</v>
       </c>
       <c r="V27" s="0" t="inlineStr">
         <is>
@@ -3833,7 +3826,7 @@
       </c>
       <c r="X27" s="0" t="inlineStr">
         <is>
-          <t>FLOOR BOARD DIRTY BY DUST.</t>
+          <t>F/B DIRTY BY DROP OIL SPOT,TYER MARK, &amp; BADLY MUD DUST.</t>
         </is>
       </c>
       <c r="Y27" s="0" t="inlineStr">
@@ -3854,19 +3847,19 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="n">
-        <v>37040</v>
+        <v>39636</v>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>IAAU2753116</t>
+          <t>IAAU1712004</t>
         </is>
       </c>
       <c r="C28" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>HC</t>
         </is>
       </c>
       <c r="E28" s="0" t="inlineStr">
@@ -3881,40 +3874,40 @@
       </c>
       <c r="G28" s="0" t="inlineStr">
         <is>
+          <t>SAPL-W</t>
+        </is>
+      </c>
+      <c r="H28" s="0" t="inlineStr">
+        <is>
           <t>SAPL-E</t>
         </is>
       </c>
-      <c r="H28" s="0" t="inlineStr">
-        <is>
-          <t>SAPL-E</t>
-        </is>
-      </c>
       <c r="I28" s="0" t="inlineStr">
         <is>
-          <t>MV.X-PRESS KOHIMA</t>
+          <t>XPRESS LHOTSE</t>
         </is>
       </c>
       <c r="J28" s="0" t="inlineStr">
         <is>
-          <t>2018/1935</t>
+          <t>2703/2018</t>
         </is>
       </c>
       <c r="K28" s="0" t="inlineStr">
         <is>
-          <t>OTC</t>
-        </is>
-      </c>
-      <c r="L28" s="0" t="d">
-        <v>2018-07-03T00:00:00</v>
-      </c>
-      <c r="M28" s="0" t="inlineStr">
-        <is>
-          <t>CLEANED</t>
-        </is>
-      </c>
-      <c r="N28" s="0"/>
+          <t>IMPORT</t>
+        </is>
+      </c>
+      <c r="L28" s="4" t="d">
+        <v>2018-09-16T00:00:00</v>
+      </c>
+      <c r="M28" s="4" t="inlineStr">
+        <is>
+          <t>DAMAGE</t>
+        </is>
+      </c>
+      <c r="N28" s="4"/>
       <c r="O28" s="0" t="n">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="P28" s="0" t="n">
         <v>0</v>
@@ -3928,21 +3921,21 @@
       <c r="S28" s="0"/>
       <c r="T28" s="0"/>
       <c r="U28" s="0" t="n">
-        <v>1447518</v>
+        <v>1480253</v>
       </c>
       <c r="V28" s="0" t="inlineStr">
         <is>
-          <t>FLOORS-(F)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W28" s="0" t="inlineStr">
         <is>
-          <t>Threshold plate-(Threshold plate)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X28" s="0" t="inlineStr">
         <is>
-          <t>FLOOR BOARD DIRTY BY DUST.</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y28" s="0" t="inlineStr">
@@ -4013,15 +4006,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L29" s="0" t="d">
+      <c r="L29" s="4" t="d">
         <v>2018-09-16T00:00:00</v>
       </c>
-      <c r="M29" s="0" t="inlineStr">
+      <c r="M29" s="4" t="inlineStr">
         <is>
           <t>DAMAGE</t>
         </is>
       </c>
-      <c r="N29" s="0"/>
+      <c r="N29" s="4"/>
       <c r="O29" s="0" t="n">
         <v>73</v>
       </c>
@@ -4041,17 +4034,17 @@
       </c>
       <c r="V29" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W29" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X29" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
         </is>
       </c>
       <c r="Y29" s="0" t="inlineStr">
@@ -4122,15 +4115,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L30" s="0" t="d">
+      <c r="L30" s="4" t="d">
         <v>2018-09-16T00:00:00</v>
       </c>
-      <c r="M30" s="0" t="inlineStr">
+      <c r="M30" s="4" t="inlineStr">
         <is>
           <t>DAMAGE</t>
         </is>
       </c>
-      <c r="N30" s="0"/>
+      <c r="N30" s="4"/>
       <c r="O30" s="0" t="n">
         <v>73</v>
       </c>
@@ -4160,7 +4153,7 @@
       </c>
       <c r="X30" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
+          <t>F/B STEEL PLATE FITTING 12'X08' &amp; LOOSED .</t>
         </is>
       </c>
       <c r="Y30" s="0" t="inlineStr">
@@ -4181,11 +4174,11 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="n">
-        <v>39636</v>
+        <v>39637</v>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>IAAU1712004</t>
+          <t>IAAU1723293</t>
         </is>
       </c>
       <c r="C31" s="0" t="n">
@@ -4231,15 +4224,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L31" s="0" t="d">
+      <c r="L31" s="4" t="d">
         <v>2018-09-16T00:00:00</v>
       </c>
-      <c r="M31" s="0" t="inlineStr">
-        <is>
-          <t>DAMAGE</t>
-        </is>
-      </c>
-      <c r="N31" s="0"/>
+      <c r="M31" s="4" t="inlineStr">
+        <is>
+          <t>WASH</t>
+        </is>
+      </c>
+      <c r="N31" s="4"/>
       <c r="O31" s="0" t="n">
         <v>73</v>
       </c>
@@ -4255,21 +4248,21 @@
       <c r="S31" s="0"/>
       <c r="T31" s="0"/>
       <c r="U31" s="0" t="n">
-        <v>1480253</v>
+        <v>1480254</v>
       </c>
       <c r="V31" s="0" t="inlineStr">
         <is>
-          <t>FLOORS-(F)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W31" s="0" t="inlineStr">
         <is>
-          <t>Threshold plate-(Threshold plate)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X31" s="0" t="inlineStr">
         <is>
-          <t>F/B STEEL PLATE FITTING 12'X08' &amp; LOOSED .</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y31" s="0" t="inlineStr">
@@ -4340,15 +4333,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L32" s="0" t="d">
+      <c r="L32" s="4" t="d">
         <v>2018-09-16T00:00:00</v>
       </c>
-      <c r="M32" s="0" t="inlineStr">
+      <c r="M32" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N32" s="0"/>
+      <c r="N32" s="4"/>
       <c r="O32" s="0" t="n">
         <v>73</v>
       </c>
@@ -4368,17 +4361,17 @@
       </c>
       <c r="V32" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W32" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X32" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
         </is>
       </c>
       <c r="Y32" s="0" t="inlineStr">
@@ -4399,11 +4392,11 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="n">
-        <v>39637</v>
+        <v>39827</v>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>IAAU1723293</t>
+          <t>IAAU1690348</t>
         </is>
       </c>
       <c r="C33" s="0" t="n">
@@ -4426,7 +4419,7 @@
       </c>
       <c r="G33" s="0" t="inlineStr">
         <is>
-          <t>SAPL-W</t>
+          <t>SAPL-E</t>
         </is>
       </c>
       <c r="H33" s="0" t="inlineStr">
@@ -4449,17 +4442,17 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L33" s="0" t="d">
-        <v>2018-09-16T00:00:00</v>
-      </c>
-      <c r="M33" s="0" t="inlineStr">
+      <c r="L33" s="4" t="d">
+        <v>2018-09-15T00:00:00</v>
+      </c>
+      <c r="M33" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N33" s="0"/>
+      <c r="N33" s="4"/>
       <c r="O33" s="0" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P33" s="0" t="n">
         <v>0</v>
@@ -4473,21 +4466,21 @@
       <c r="S33" s="0"/>
       <c r="T33" s="0"/>
       <c r="U33" s="0" t="n">
-        <v>1480254</v>
+        <v>1480608</v>
       </c>
       <c r="V33" s="0" t="inlineStr">
         <is>
-          <t>FLOORS-(F)</t>
+          <t>PANELS-(PANELS)</t>
         </is>
       </c>
       <c r="W33" s="0" t="inlineStr">
         <is>
-          <t>Threshold plate-(Threshold plate)</t>
+          <t>Right side panel -(Right side panel )</t>
         </is>
       </c>
       <c r="X33" s="0" t="inlineStr">
         <is>
-          <t>F/B DIRTY BY MUD,DROP OIL SPOT,TYER MARK,SAND ,SATPLE FIBER DUST .</t>
+          <t>INTERNAL PANEL DIRTY.</t>
         </is>
       </c>
       <c r="Y33" s="0" t="inlineStr">
@@ -4558,15 +4551,15 @@
           <t>IMPORT</t>
         </is>
       </c>
-      <c r="L34" s="0" t="d">
+      <c r="L34" s="4" t="d">
         <v>2018-09-15T00:00:00</v>
       </c>
-      <c r="M34" s="0" t="inlineStr">
+      <c r="M34" s="4" t="inlineStr">
         <is>
           <t>WASH</t>
         </is>
       </c>
-      <c r="N34" s="0"/>
+      <c r="N34" s="4"/>
       <c r="O34" s="0" t="n">
         <v>74</v>
       </c>
@@ -4586,17 +4579,17 @@
       </c>
       <c r="V34" s="0" t="inlineStr">
         <is>
-          <t>PANELS-(PANELS)</t>
+          <t>FLOORS-(F)</t>
         </is>
       </c>
       <c r="W34" s="0" t="inlineStr">
         <is>
-          <t>Right side panel -(Right side panel )</t>
+          <t>Threshold plate-(Threshold plate)</t>
         </is>
       </c>
       <c r="X34" s="0" t="inlineStr">
         <is>
-          <t>INTERNAL PANEL DIRTY.</t>
+          <t>F/B DIRTY BY BADLY MUD+SAND,TYER MARK STAPLE FIBER DUST &amp; ODOUR</t>
         </is>
       </c>
       <c r="Y34" s="0" t="inlineStr">
@@ -4610,115 +4603,6 @@
         </is>
       </c>
       <c r="AA34" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="0" t="n">
-        <v>39827</v>
-      </c>
-      <c r="B35" s="0" t="inlineStr">
-        <is>
-          <t>IAAU1690348</t>
-        </is>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="D35" s="0" t="inlineStr">
-        <is>
-          <t>HC</t>
-        </is>
-      </c>
-      <c r="E35" s="0" t="inlineStr">
-        <is>
-          <t>BS</t>
-        </is>
-      </c>
-      <c r="F35" s="0" t="inlineStr">
-        <is>
-          <t>ICB</t>
-        </is>
-      </c>
-      <c r="G35" s="0" t="inlineStr">
-        <is>
-          <t>SAPL-E</t>
-        </is>
-      </c>
-      <c r="H35" s="0" t="inlineStr">
-        <is>
-          <t>SAPL-E</t>
-        </is>
-      </c>
-      <c r="I35" s="0" t="inlineStr">
-        <is>
-          <t>XPRESS LHOTSE</t>
-        </is>
-      </c>
-      <c r="J35" s="0" t="inlineStr">
-        <is>
-          <t>2703/2018</t>
-        </is>
-      </c>
-      <c r="K35" s="0" t="inlineStr">
-        <is>
-          <t>IMPORT</t>
-        </is>
-      </c>
-      <c r="L35" s="0" t="d">
-        <v>2018-09-15T00:00:00</v>
-      </c>
-      <c r="M35" s="0" t="inlineStr">
-        <is>
-          <t>WASH</t>
-        </is>
-      </c>
-      <c r="N35" s="0"/>
-      <c r="O35" s="0" t="n">
-        <v>74</v>
-      </c>
-      <c r="P35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="0" t="inlineStr">
-        <is>
-          <t>Empty</t>
-        </is>
-      </c>
-      <c r="R35" s="0"/>
-      <c r="S35" s="0"/>
-      <c r="T35" s="0"/>
-      <c r="U35" s="0" t="n">
-        <v>1480608</v>
-      </c>
-      <c r="V35" s="0" t="inlineStr">
-        <is>
-          <t>FLOORS-(F)</t>
-        </is>
-      </c>
-      <c r="W35" s="0" t="inlineStr">
-        <is>
-          <t>Threshold plate-(Threshold plate)</t>
-        </is>
-      </c>
-      <c r="X35" s="0" t="inlineStr">
-        <is>
-          <t>F/B DIRTY BY BADLY MUD+SAND,TYER MARK STAPLE FIBER DUST &amp; ODOUR</t>
-        </is>
-      </c>
-      <c r="Y35" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="Z35" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AA35" s="0" t="inlineStr">
         <is>
           <t/>
         </is>
@@ -4745,23 +4629,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="75.25617977528091" hidden="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.8561797752809" hidden="false"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.213483146067416"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.713483146067418"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="10.213483146067416"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="7.213483146067416"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.713483146067416"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="8.713483146067416"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="7.213483146067416"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.713483146067416"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.213483146067416"/>
   </cols>
   <sheetData>
     <row ht="20" customHeight="true" r="1">
@@ -4771,78 +4655,117 @@
         </is>
       </c>
     </row>
-    <row ht="18" customHeight="true" r="2">
+    <row ht="16" customHeight="true" r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t> KATGHAR, NORTH PATENGA, CHITTAGONG-4204. </t>
-        </is>
-      </c>
-    </row>
-    <row ht="16" customHeight="true" r="3">
+          <t>ICB</t>
+        </is>
+      </c>
+    </row>
+    <row ht="14" customHeight="true" r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
+          <t>Stock Report Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Mlo</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Container Size Type</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>Sound</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>Repaired</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>Damage</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>Wash</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>Sweep</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
+          <t>Clean</t>
+        </is>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>Total Box</t>
+        </is>
+      </c>
+      <c r="K5" s="5" t="inlineStr">
+        <is>
+          <t>Total Teus</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>BS</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
           <t>ICB</t>
         </is>
       </c>
-    </row>
-    <row ht="14" customHeight="true" r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>Stock Report Summary</t>
-        </is>
-      </c>
-    </row>
-    <row r="5"/>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Agent</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>MLO</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>Size-Type</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>Sound</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>Repaired</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr">
-        <is>
-          <t>Damage</t>
-        </is>
-      </c>
-      <c r="G6" s="4" t="inlineStr">
-        <is>
-          <t>Wash</t>
-        </is>
-      </c>
-      <c r="H6" s="4" t="inlineStr">
-        <is>
-          <t>Sweep</t>
-        </is>
-      </c>
-      <c r="I6" s="4" t="inlineStr">
-        <is>
-          <t>Clean</t>
-        </is>
-      </c>
-      <c r="J6" s="4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>20-GP</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -4858,7 +4781,7 @@
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>20-GP</t>
+          <t>40-HC</t>
         </is>
       </c>
       <c r="D7" s="0" t="n">
@@ -4868,62 +4791,21 @@
         <v>0</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="inlineStr">
-        <is>
-          <t>BS</t>
-        </is>
-      </c>
-      <c r="B8" s="0" t="inlineStr">
-        <is>
-          <t>ICB</t>
-        </is>
-      </c>
-      <c r="C8" s="0" t="inlineStr">
-        <is>
-          <t>40-HC</t>
-        </is>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="K8" s="0" t="n">
         <v>26</v>
       </c>
     </row>

</xml_diff>